<commit_message>
No changes, just saved file
</commit_message>
<xml_diff>
--- a/workedexample/Matt Mazur Example.xlsx
+++ b/workedexample/Matt Mazur Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuar\Documents\sw-dev\simple-neural-network\workedexample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56C92510-B02C-443F-BF67-3B3304434CD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5864B26-E00A-4BD6-9782-456707542B94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="1575" windowWidth="22860" windowHeight="13980" xr2:uid="{A2271C3C-57FA-4F44-BB9E-6D440CBB85AF}"/>
   </bookViews>
@@ -3333,7 +3333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA31DF84-8569-4304-A9EF-BD1D3F4E345B}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>

</xml_diff>